<commit_message>
S senditivity added to the function
</commit_message>
<xml_diff>
--- a/CVX_Kenya/my_graphs/CO2 Change by Activities.xlsx
+++ b/CVX_Kenya/my_graphs/CO2 Change by Activities.xlsx
@@ -453,19 +453,19 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>-3.849871493266654E-06</v>
+        <v>2.232981138561296E-05</v>
       </c>
       <c r="D2">
-        <v>-0.0007587638362167581</v>
+        <v>0.004400939973805862</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>-3.849871493266654E-06</v>
+        <v>2.232981138561296E-05</v>
       </c>
       <c r="G2">
-        <v>-1.924935746666634E-05</v>
+        <v>0.0001116490569281758</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -476,19 +476,19 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>-5.723379266520112E-05</v>
+        <v>3.276756976866579E-09</v>
       </c>
       <c r="D3">
-        <v>-0.0002289351706608045</v>
+        <v>1.310702790746632E-08</v>
       </c>
       <c r="E3">
-        <v>-6.997814285325532E-05</v>
+        <v>4.006398324207794E-09</v>
       </c>
       <c r="F3">
-        <v>-0.0001060881644852074</v>
+        <v>6.073774150294753E-09</v>
       </c>
       <c r="G3">
-        <v>-0.0002861689633260056</v>
+        <v>1.63837849953552E-08</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -499,19 +499,19 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>-3.645935777924804E-06</v>
+        <v>1.054685679069411E-11</v>
       </c>
       <c r="D4">
-        <v>-1.458374311169922E-05</v>
+        <v>4.218742716277646E-11</v>
       </c>
       <c r="E4">
-        <v>-0.01667553575848046</v>
+        <v>4.823850474622304E-08</v>
       </c>
       <c r="F4">
-        <v>-0.002696648351875552</v>
+        <v>7.800784906919489E-09</v>
       </c>
       <c r="G4">
-        <v>-1.822967888962662E-05</v>
+        <v>5.27342822187471E-11</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -522,19 +522,19 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>-0.0007856804454604571</v>
+        <v>0.07578661345678483</v>
       </c>
       <c r="D5">
-        <v>-1.319636495633603E-06</v>
+        <v>0.0001272919309522891</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>-3.299091239084007E-07</v>
+        <v>3.182298273807227E-05</v>
       </c>
       <c r="G5">
-        <v>-1.649545619208936E-06</v>
+        <v>0.0001591149136901393</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -545,19 +545,19 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>-6.490797254093961E-06</v>
+        <v>1.478532157817014E-08</v>
       </c>
       <c r="D6">
-        <v>-0.001279258861803356</v>
+        <v>2.914010849508486E-06</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>-6.490797254093961E-06</v>
+        <v>1.478532157817014E-08</v>
       </c>
       <c r="G6">
-        <v>-3.245398627049756E-05</v>
+        <v>7.392660783533955E-08</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -568,19 +568,19 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>-6.741214118866079E-08</v>
+        <v>1.930840100305975E-08</v>
       </c>
       <c r="D7">
-        <v>-2.696485647546432E-07</v>
+        <v>7.7233604012239E-08</v>
       </c>
       <c r="E7">
-        <v>-0.0003083251158955136</v>
+        <v>8.83114652765471E-05</v>
       </c>
       <c r="F7">
-        <v>-4.986013207286533E-05</v>
+        <v>1.428109840162506E-05</v>
       </c>
       <c r="G7">
-        <v>-3.370607059016706E-07</v>
+        <v>9.654200505693211E-08</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -588,22 +588,22 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>-0.001442674993313631</v>
+        <v>0.00330747736916237</v>
       </c>
       <c r="C8">
-        <v>-2.295143349151374E-06</v>
+        <v>0.0004874692202960773</v>
       </c>
       <c r="D8">
-        <v>-0.0002106254291902587</v>
+        <v>0.08780026868078039</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>-2.295143349151374E-06</v>
+        <v>0.0004874692202960773</v>
       </c>
       <c r="G8">
-        <v>-1.147571674664505E-05</v>
+        <v>0.002437346101480387</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -614,19 +614,19 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>-4.582789647766816E-08</v>
+        <v>1.342734235232346E-05</v>
       </c>
       <c r="D9">
-        <v>-3.948826599753374E-05</v>
+        <v>0.01156986263652016</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>-4.582789647766816E-08</v>
+        <v>1.342734235232346E-05</v>
       </c>
       <c r="G9">
-        <v>-2.291394824993631E-07</v>
+        <v>6.713671176150626E-05</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -637,19 +637,19 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>-0.0003281661049001627</v>
+        <v>3.994091957792989E-05</v>
       </c>
       <c r="D10">
-        <v>-0.001314782937697601</v>
+        <v>0.003533260433755459</v>
       </c>
       <c r="E10">
-        <v>-0.003146433185435171</v>
+        <v>1.500819767841222E-05</v>
       </c>
       <c r="F10">
-        <v>-0.002522570590627993</v>
+        <v>5.412836907225937E-05</v>
       </c>
       <c r="G10">
-        <v>-0.001640830524507919</v>
+        <v>0.0001997045978896494</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -660,19 +660,19 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>6.047599214298316E-06</v>
+        <v>7.279715729779923E-06</v>
       </c>
       <c r="D11">
-        <v>-0.0005253112240097835</v>
+        <v>0.001560155710080835</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>-0.0001463899232021504</v>
+        <v>0.0006627228178786027</v>
       </c>
       <c r="G11">
-        <v>-0.01139014543241501</v>
+        <v>0.01782423959866719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on units for plot_ds matrix
</commit_message>
<xml_diff>
--- a/CVX_Kenya/my_graphs/CO2 Change by Activities.xlsx
+++ b/CVX_Kenya/my_graphs/CO2 Change by Activities.xlsx
@@ -14,54 +14,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Cement production</t>
-  </si>
-  <si>
-    <t>Electricity and Heat</t>
-  </si>
-  <si>
-    <t>Industry</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Residential</t>
-  </si>
-  <si>
-    <t>Transport</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>INFORMAL</t>
+  </si>
+  <si>
+    <t>COOPERATIVES</t>
+  </si>
+  <si>
+    <t>PRIMARY</t>
+  </si>
+  <si>
+    <t>COFFEE ESTATE</t>
+  </si>
+  <si>
+    <t>MANUFACTURING</t>
+  </si>
+  <si>
+    <t>PETROLEUM PROD</t>
   </si>
   <si>
     <t>CHEMICAL PROD</t>
   </si>
   <si>
-    <t>COFFEE ESTATE</t>
-  </si>
-  <si>
-    <t>COOPERATIVES</t>
+    <t>FERTILIZERS PROD</t>
   </si>
   <si>
     <t>ELECTRICITY PROD</t>
   </si>
   <si>
-    <t>FERTILIZERS PROD</t>
-  </si>
-  <si>
-    <t>INFORMAL</t>
-  </si>
-  <si>
-    <t>MANUFACTURING</t>
-  </si>
-  <si>
-    <t>PETROLEUM PROD</t>
-  </si>
-  <si>
-    <t>PRIMARY</t>
-  </si>
-  <si>
     <t>SERVICES</t>
+  </si>
+  <si>
+    <t>CO2</t>
   </si>
 </sst>
 </file>
@@ -419,263 +407,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>2.232981138561296E-05</v>
-      </c>
-      <c r="D2">
-        <v>0.004400939973805862</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>2.232981138561296E-05</v>
-      </c>
-      <c r="G2">
-        <v>0.0001116490569281758</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>3.276756976866579E-09</v>
-      </c>
-      <c r="D3">
-        <v>1.310702790746632E-08</v>
-      </c>
-      <c r="E3">
-        <v>4.006398324207794E-09</v>
-      </c>
-      <c r="F3">
-        <v>6.073774150294753E-09</v>
-      </c>
-      <c r="G3">
-        <v>1.63837849953552E-08</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.0001031120239076699</v>
       </c>
       <c r="C4">
-        <v>1.054685679069411E-11</v>
+        <v>5.675015302131214E-08</v>
       </c>
       <c r="D4">
-        <v>4.218742716277646E-11</v>
+        <v>0.003842762885369666</v>
       </c>
       <c r="E4">
-        <v>4.823850474622304E-08</v>
+        <v>4.324439117908696E-08</v>
       </c>
       <c r="F4">
-        <v>7.800784906919489E-09</v>
+        <v>0.09455534542507849</v>
       </c>
       <c r="G4">
-        <v>5.27342822187471E-11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0.07578661345678483</v>
-      </c>
-      <c r="D5">
-        <v>0.0001272919309522891</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>3.182298273807227E-05</v>
-      </c>
-      <c r="G5">
-        <v>0.0001591149136901393</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>1.478532157817014E-08</v>
-      </c>
-      <c r="D6">
-        <v>2.914010849508486E-06</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1.478532157817014E-08</v>
-      </c>
-      <c r="G6">
-        <v>7.392660783533955E-08</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1.930840100305975E-08</v>
-      </c>
-      <c r="D7">
-        <v>7.7233604012239E-08</v>
-      </c>
-      <c r="E7">
-        <v>8.83114652765471E-05</v>
-      </c>
-      <c r="F7">
-        <v>1.428109840162506E-05</v>
-      </c>
-      <c r="G7">
-        <v>9.654200505693211E-08</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>0.00330747736916237</v>
-      </c>
-      <c r="C8">
-        <v>0.0004874692202960773</v>
-      </c>
-      <c r="D8">
-        <v>0.08780026868078039</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0.0004874692202960773</v>
-      </c>
-      <c r="G8">
-        <v>0.002437346101480387</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>1.342734235232346E-05</v>
-      </c>
-      <c r="D9">
-        <v>0.01156986263652016</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>1.342734235232346E-05</v>
-      </c>
-      <c r="G9">
-        <v>6.713671176150626E-05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>3.994091957792989E-05</v>
-      </c>
-      <c r="D10">
-        <v>0.003533260433755459</v>
-      </c>
-      <c r="E10">
-        <v>1.500819767841222E-05</v>
-      </c>
-      <c r="F10">
-        <v>5.412836907225937E-05</v>
-      </c>
-      <c r="G10">
-        <v>0.0001997045978896494</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>7.279715729779923E-06</v>
-      </c>
-      <c r="D11">
-        <v>0.001560155710080835</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0.0006627228178786027</v>
-      </c>
-      <c r="G11">
-        <v>0.01782423959866719</v>
+        <v>0.01170050304563119</v>
+      </c>
+      <c r="H4">
+        <v>0.004558103997425178</v>
+      </c>
+      <c r="I4">
+        <v>3.027877522043809E-06</v>
+      </c>
+      <c r="J4">
+        <v>0.07615523642971311</v>
+      </c>
+      <c r="K4">
+        <v>0.02022164995378262</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
plot issues solved, unit of ds fixed automatically
</commit_message>
<xml_diff>
--- a/CVX_Kenya/my_graphs/CO2 Change by Activities.xlsx
+++ b/CVX_Kenya/my_graphs/CO2 Change by Activities.xlsx
@@ -14,42 +14,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Activities</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Cement production</t>
+  </si>
+  <si>
+    <t>Electricity and Heat</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>CHEMICAL PROD</t>
+  </si>
+  <si>
+    <t>COFFEE ESTATE</t>
+  </si>
+  <si>
+    <t>COOPERATIVES</t>
+  </si>
+  <si>
+    <t>ELECTRICITY PROD</t>
+  </si>
+  <si>
+    <t>FERTILIZERS PROD</t>
   </si>
   <si>
     <t>INFORMAL</t>
   </si>
   <si>
-    <t>COOPERATIVES</t>
+    <t>MANUFACTURING</t>
+  </si>
+  <si>
+    <t>PETROLEUM PROD</t>
   </si>
   <si>
     <t>PRIMARY</t>
   </si>
   <si>
-    <t>COFFEE ESTATE</t>
-  </si>
-  <si>
-    <t>MANUFACTURING</t>
-  </si>
-  <si>
-    <t>PETROLEUM PROD</t>
-  </si>
-  <si>
-    <t>CHEMICAL PROD</t>
-  </si>
-  <si>
-    <t>FERTILIZERS PROD</t>
-  </si>
-  <si>
-    <t>ELECTRICITY PROD</t>
-  </si>
-  <si>
     <t>SERVICES</t>
-  </si>
-  <si>
-    <t>CO2</t>
   </si>
 </sst>
 </file>
@@ -407,99 +419,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>2.233400243811801E-05</v>
+      </c>
+      <c r="D2">
+        <v>0.004401765980361461</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2.233400243811801E-05</v>
+      </c>
+      <c r="G2">
+        <v>0.00011167001219059</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>3.30709060136769E-09</v>
+      </c>
+      <c r="D3">
+        <v>1.322836240547076E-08</v>
+      </c>
+      <c r="E3">
+        <v>4.043486212523817E-09</v>
+      </c>
+      <c r="F3">
+        <v>6.130000285153869E-09</v>
+      </c>
+      <c r="G3">
+        <v>1.653545300683845E-08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1.066058092497046E-11</v>
+      </c>
+      <c r="D4">
+        <v>4.264232369988186E-11</v>
+      </c>
+      <c r="E4">
+        <v>4.875864334508151E-08</v>
+      </c>
+      <c r="F4">
+        <v>7.88489895597877E-09</v>
+      </c>
+      <c r="G4">
+        <v>5.330290375749058E-11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.07583679588196901</v>
+      </c>
+      <c r="D5">
+        <v>0.0001273762178408688</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>3.184405446021721E-05</v>
+      </c>
+      <c r="G5">
+        <v>0.000159220272300864</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1.483613017161378E-08</v>
+      </c>
+      <c r="D6">
+        <v>2.924024627759536E-06</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1.483613017161378E-08</v>
+      </c>
+      <c r="G6">
+        <v>7.418065084419112E-08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>0.0001031120239076699</v>
-      </c>
-      <c r="C4">
-        <v>5.675015302131214E-08</v>
-      </c>
-      <c r="D4">
-        <v>0.003842762885369666</v>
-      </c>
-      <c r="E4">
-        <v>4.324439117908696E-08</v>
-      </c>
-      <c r="F4">
-        <v>0.09455534542507849</v>
-      </c>
-      <c r="G4">
-        <v>0.01170050304563119</v>
-      </c>
-      <c r="H4">
-        <v>0.004558103997425178</v>
-      </c>
-      <c r="I4">
-        <v>3.027877522043809E-06</v>
-      </c>
-      <c r="J4">
-        <v>0.07615523642971311</v>
-      </c>
-      <c r="K4">
-        <v>0.02022164995378262</v>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1.936971111282659E-08</v>
+      </c>
+      <c r="D7">
+        <v>7.747884445130637E-08</v>
+      </c>
+      <c r="E7">
+        <v>8.859188142196217E-05</v>
+      </c>
+      <c r="F7">
+        <v>1.432644531007554E-05</v>
+      </c>
+      <c r="G7">
+        <v>9.684855556413297E-08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>0.003331653041414029</v>
+      </c>
+      <c r="C8">
+        <v>0.0004876032706917499</v>
+      </c>
+      <c r="D8">
+        <v>0.08781046948865878</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.0004876032706917499</v>
+      </c>
+      <c r="G8">
+        <v>0.00243801635345875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1.34695324246481E-05</v>
+      </c>
+      <c r="D9">
+        <v>0.01160621631879621</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1.34695324246481E-05</v>
+      </c>
+      <c r="G9">
+        <v>6.734766212357357E-05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>3.998540645966386E-05</v>
+      </c>
+      <c r="D10">
+        <v>0.003533529941023517</v>
+      </c>
+      <c r="E10">
+        <v>1.507383637999737E-05</v>
+      </c>
+      <c r="F10">
+        <v>5.424666913711462E-05</v>
+      </c>
+      <c r="G10">
+        <v>0.0001999270322983193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>7.764378329611077E-06</v>
+      </c>
+      <c r="D11">
+        <v>0.00157231138109637</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.0007004048203498314</v>
+      </c>
+      <c r="G11">
+        <v>0.01794116937071522</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:K1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>